<commit_message>
chd normal corr 45
</commit_message>
<xml_diff>
--- a/chd_tests/chd_grid_Q_Normal.xlsx
+++ b/chd_tests/chd_grid_Q_Normal.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,6 +700,586 @@
         <v>0.3753441990568563</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.080166504188284</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-1.390476677927515</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.2980841856143616</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.471029234077814</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.3747115521091721</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.8994690427722825</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-1.398574963125803</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.2952507445860527</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.4712791868485272</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.3736449071541705</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.4261995378958547</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-1.421233767473362</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.2901329598009249</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.4707988478433893</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.3687079851421951</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-0.1293866511906445</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-1.445894254428907</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.2881183117335868</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.4634287222226601</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3671734660080277</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.2056862336605694</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-1.431506400279586</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.2916483634698089</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.4621820912026547</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3668967082701994</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-0.1867035728334181</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-1.449493393027206</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.2920552357523991</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.4634912525595197</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3664404882586997</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-0.6440158654643769</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.469374742207627</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.2927357270699735</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.476967520816862</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.3660762421732142</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-1.00310434740966</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-1.486577319749939</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.2823257794302023</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.4573051486249445</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.3609390017017186</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>-1.504651547717967</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-1.504352060833916</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.2824063043884478</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.4673525213334017</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.3589114020489111</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>-1.523057165276164</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-1.506251585126765</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.2874913509468727</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.4763186895251477</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.3596254387762725</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>-1.547866526217289</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-1.505981936801861</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.2824917548237356</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.470297959717995</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.3590407684702159</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>-1.674789248526957</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-1.515261708185203</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.2810911706267988</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.4598718992479331</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.3565231970190204</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>-1.80887009342756</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-1.519719238190314</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.2817731283685904</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.4628821637453638</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.3563924736662875</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.959006920876836</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-1.528575197003926</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.283096887754046</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.468178751116758</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.3569955320223329</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>-2.628002259608796</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-1.556738706060644</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.2797088712910335</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.4619532977942937</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.3538870764782091</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-2.74519343513492</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-1.562936471518154</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.2829719137906281</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.4693568661235901</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.3539594814604756</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>-2.616699140309548</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-1.555467643488537</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.2817799361924212</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.4678291031621125</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.354810156502578</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-2.791589609579778</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-1.566469941565195</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.2797834832899018</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.4643306684375735</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.354365384517229</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>-3.652310185618549</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-1.60261055199894</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.2759074987536526</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.4603970618121689</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.3493041882624723</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>-3.756174605209603</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-1.606526802227228</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.2739302211430541</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.4620109193277304</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.3478127771358528</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>-2.882811803245962</v>
+      </c>
+      <c r="C34" t="n">
+        <v>-1.568264211766325</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.2801776300458057</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.4677487387920243</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.352676499971505</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>-3.528348743073225</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-1.597079792213081</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.281630330223537</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.4703283830767131</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.3537166474006844</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-4.244336103330546</v>
+      </c>
+      <c r="C36" t="n">
+        <v>-1.629060565180591</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.2744093277546549</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.4653617167751883</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.3472367264797188</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>-4.071438086209068</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-1.621458705173424</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.2742760764748384</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.4607637103988677</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.3465295138439479</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>-4.15268585930187</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-1.623869896395521</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.2785705132622892</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.4633721880379841</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.3474495646371155</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>-4.00014195331548</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-1.616895041109092</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.2782202908540612</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.4726757433231457</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.3518676810744165</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>-5.025020935305634</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-1.663951270060294</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.2764851337111826</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.4634239827650745</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.3434005295085088</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>-5.250027027656023</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-1.671895129287924</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.2698112294118212</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.4640487639547825</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.3419727282231946</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>-4.610919432025785</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-1.645522452663342</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.2751076341681803</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.4628541490318563</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.3473471770533686</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
advance in lmc 36
</commit_message>
<xml_diff>
--- a/chd_tests/chd_grid_Q_Normal.xlsx
+++ b/chd_tests/chd_grid_Q_Normal.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,82 +462,182 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B2" t="n">
-        <v>39.51091011845141</v>
+        <v>0.8107328646344186</v>
       </c>
       <c r="C2" t="n">
-        <v>3.330194587715765</v>
+        <v>-1.404552951823922</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2757206529720492</v>
+        <v>0.2791825964964812</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09693213456195145</v>
+        <v>0.4642850981975821</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2200127669425106</v>
+        <v>0.3576535517144857</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B3" t="n">
-        <v>31.82357426535455</v>
+        <v>1.197979265296577</v>
       </c>
       <c r="C3" t="n">
-        <v>2.851496968809787</v>
+        <v>-1.383524806554267</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2642692414907299</v>
+        <v>0.2793392705239028</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1597622971544773</v>
+        <v>0.4611815990091802</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3018524677357201</v>
+        <v>0.3560022500362016</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" t="n">
-        <v>34.2398078577875</v>
+        <v>5.555209259952779</v>
       </c>
       <c r="C4" t="n">
-        <v>2.985300181131098</v>
+        <v>-1.196796697727143</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2374212359492403</v>
+        <v>0.295648926262209</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1457039933828208</v>
+        <v>0.4756433605480084</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2795570754040665</v>
+        <v>0.3792873153245865</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B5" t="n">
-        <v>30.85518531110552</v>
+        <v>2.024697424499826</v>
       </c>
       <c r="C5" t="n">
-        <v>2.908898957494153</v>
+        <v>-1.349387073041513</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2367088376218902</v>
+        <v>0.283575169927707</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1348696722909579</v>
+        <v>0.457505340064679</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2640533844208901</v>
+        <v>0.3643838030461788</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9735009822949687</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-1.39625761291196</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2752441701796778</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.4556972671299721</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.3559362525705976</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-0.9126926661758791</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-1.48086255930799</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.2741533070165214</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.4606079045795512</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3501436751722561</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.231027972550454</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1.341482471523983</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.2807881996020219</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.4612579830966981</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3624319567207067</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.2549752556816626</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-1.425702310784218</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2751145571388615</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.4613300348097312</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.3534310911770412</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B10" t="n">
+        <v>4.474318729867433</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-1.239134840997663</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.2877082482069251</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.4638503111729836</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.3705068175371698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ending with chd lmc normal
</commit_message>
<xml_diff>
--- a/chd_tests/chd_grid_Q_Normal.xlsx
+++ b/chd_tests/chd_grid_Q_Normal.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,182 +462,222 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8107328646344186</v>
+        <v>2.123996793003155</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.404552951823922</v>
+        <v>-1.341851536611955</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2791825964964812</v>
+        <v>0.2826872811415794</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4642850981975821</v>
+        <v>0.4676428022577083</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3576535517144857</v>
+        <v>0.3615278921897729</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B3" t="n">
-        <v>1.197979265296577</v>
+        <v>2.999549018034927</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.383524806554267</v>
+        <v>-1.305966639919423</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2793392705239028</v>
+        <v>0.2789175382363926</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4611815990091802</v>
+        <v>0.4622694510566538</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3560022500362016</v>
+        <v>0.3606330597665377</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B4" t="n">
-        <v>5.555209259952779</v>
+        <v>2.006392134354136</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.196796697727143</v>
+        <v>-1.342358922876254</v>
       </c>
       <c r="D4" t="n">
-        <v>0.295648926262209</v>
+        <v>0.2780857581067647</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4756433605480084</v>
+        <v>0.4626607278200771</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3792873153245865</v>
+        <v>0.3603571426381924</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B5" t="n">
-        <v>2.024697424499826</v>
+        <v>3.240696515968457</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.349387073041513</v>
+        <v>-1.295640757642037</v>
       </c>
       <c r="D5" t="n">
-        <v>0.283575169927707</v>
+        <v>0.2802419799738735</v>
       </c>
       <c r="E5" t="n">
-        <v>0.457505340064679</v>
+        <v>0.4654042137349904</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3643838030461788</v>
+        <v>0.3627833696019208</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9735009822949687</v>
+        <v>3.730790296199632</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.39625761291196</v>
+        <v>-1.274821990365726</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2752441701796778</v>
+        <v>0.2861881056395761</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4556972671299721</v>
+        <v>0.4688292432995688</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3559362525705976</v>
+        <v>0.3644847951351571</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.9126926661758791</v>
+        <v>7.168579958009738</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.48086255930799</v>
+        <v>-1.124017827048016</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2741533070165214</v>
+        <v>0.2972256193218946</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4606079045795512</v>
+        <v>0.4943963225100994</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3501436751722561</v>
+        <v>0.3866122479142569</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B8" t="n">
-        <v>2.231027972550454</v>
+        <v>6.238961826588797</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.341482471523983</v>
+        <v>-1.164018083528414</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2807881996020219</v>
+        <v>0.293609252693852</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4612579830966981</v>
+        <v>0.4761356968837653</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3624319567207067</v>
+        <v>0.3778501832234241</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2549752556816626</v>
+        <v>0.5746675060904044</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.425702310784218</v>
+        <v>-1.410359791612187</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2751145571388615</v>
+        <v>0.2727731295019905</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4613300348097312</v>
+        <v>0.4610450423698221</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3534310911770412</v>
+        <v>0.3518740037090754</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B10" t="n">
-        <v>4.474318729867433</v>
+        <v>11.18770091948372</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.239134840997663</v>
+        <v>-0.9351897937297551</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2877082482069251</v>
+        <v>0.3124566566827671</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4638503111729836</v>
+        <v>0.5171976521000549</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3705068175371698</v>
+        <v>0.4083378066995465</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3.454749111365462</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-1.286853781347119</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.2846692163941658</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.4718034380622428</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3670012483452475</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B12" t="n">
+        <v>10.74914869260767</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-0.967016390682338</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.3101819694086514</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.5107950315223438</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.4046876801675777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>